<commit_message>
even more messing up and fixing connections
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F054D4C1-AB1C-4400-A263-4A47CF1663CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF1A0A7-1AE1-4F52-A582-A9CA59D51CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1415,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="19">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="6">
         <v>0</v>
@@ -1791,6 +1791,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -1934,35 +1949,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1984,9 +1974,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added the first draft of the car times
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF1A0A7-1AE1-4F52-A582-A9CA59D51CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864DF719-2A8A-4682-9A17-E35EAE81C79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -661,7 +661,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1791,21 +1791,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -1949,10 +1934,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1974,19 +1984,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finished adding the dataframes and slight bug fixes in the excel sheets
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E199F282-532C-477C-8A6B-742C3F80A6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D6F56-F950-4E6F-9959-D1084384D31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="3560" windowWidth="19170" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,11 +524,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:Y1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -796,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="5">
         <v>0</v>
@@ -1020,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
applying exceptions within rotterdam for the car corrections in travel time
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_adjacency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D6F56-F950-4E6F-9959-D1084384D31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1E6B11-8118-4C40-86E4-2DCAC4F59562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,12 +525,12 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>